<commit_message>
take out hydro growth
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Colorado\CO_Model\InputData\elec\MCGLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9F1CE0-80EF-4CFB-9D1F-BFC048A6C89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3FE78D-DBF7-4E7F-A670-EEB396E96997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20160" windowHeight="14730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="6" r:id="rId1"/>
@@ -1592,7 +1592,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,12 +1710,11 @@
         <v>118</v>
       </c>
       <c r="C8" s="13">
-        <f t="shared" ref="C8" si="1">$C$2</f>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="D8" s="11">
         <f>C8</f>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1753,7 +1752,7 @@
         <v>118</v>
       </c>
       <c r="C10" s="13">
-        <f t="shared" ref="C10" si="2">$C$2</f>
+        <f t="shared" ref="C10" si="1">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D10" s="13">
@@ -1821,7 +1820,7 @@
         <v>118</v>
       </c>
       <c r="C12" s="13">
-        <f t="shared" ref="C12" si="3">$C$2</f>
+        <f t="shared" ref="C12" si="2">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D12" s="13">
@@ -1916,7 +1915,7 @@
         <v>118</v>
       </c>
       <c r="C14" s="13">
-        <f t="shared" ref="C14" si="4">$C$2</f>
+        <f t="shared" ref="C14" si="3">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D14" s="11">
@@ -1944,7 +1943,7 @@
         <v>118</v>
       </c>
       <c r="C16" s="13">
-        <f t="shared" ref="C16" si="5">$C$2</f>
+        <f t="shared" ref="C16" si="4">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D16" s="11">
@@ -1972,7 +1971,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="13">
-        <f t="shared" ref="C18" si="6">$C$2</f>
+        <f t="shared" ref="C18" si="5">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D18" s="11">
@@ -2000,7 +1999,7 @@
         <v>118</v>
       </c>
       <c r="C20" s="13">
-        <f t="shared" ref="C20" si="7">$C$2</f>
+        <f t="shared" ref="C20" si="6">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D20" s="11">
@@ -2028,7 +2027,7 @@
         <v>118</v>
       </c>
       <c r="C22" s="13">
-        <f t="shared" ref="C22" si="8">$C$2</f>
+        <f t="shared" ref="C22" si="7">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D22" s="11">
@@ -2056,7 +2055,7 @@
         <v>118</v>
       </c>
       <c r="C24" s="13">
-        <f t="shared" ref="C24" si="9">$C$2</f>
+        <f t="shared" ref="C24" si="8">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D24" s="5">
@@ -2115,7 +2114,7 @@
         <v>118</v>
       </c>
       <c r="C28" s="13">
-        <f t="shared" ref="C28" si="10">$C$2</f>
+        <f t="shared" ref="C28" si="9">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D28" s="11">
@@ -2142,7 +2141,7 @@
         <v>118</v>
       </c>
       <c r="C30" s="13">
-        <f t="shared" ref="C30" si="11">$C$2</f>
+        <f t="shared" ref="C30" si="10">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D30" s="11">
@@ -2169,7 +2168,7 @@
         <v>118</v>
       </c>
       <c r="C32" s="13">
-        <f t="shared" ref="C32" si="12">$C$2</f>
+        <f t="shared" ref="C32" si="11">$C$2</f>
         <v>3000</v>
       </c>
       <c r="D32" s="11">

</xml_diff>